<commit_message>
[CAN2-16] TLD Reqs Rev1 ready for review per [CAN2-24]
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/top_level_requirements_eric.xlsx
+++ b/Life_Cycle_Data/top_level_requirements_eric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010371\Documents\Can Controller\Reqs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D85D97-466F-4B93-8854-30C514368A51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C23593-0996-4DF3-919B-AA37F9AA7B38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{476FB2D9-C995-4132-A432-09B426472DB8}"/>
   </bookViews>
@@ -52,30 +52,6 @@
   </si>
   <si>
     <t>Initialization</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Microcontroller Bus Interface as DUT0.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Configuration Registers as DUT1.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Rx FIFO as DUT3.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Tx FIFO as DUT2.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Tx Priority Logic as DUT4.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Acceptance Filter as DUT5.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Bit Stream Processor as DUT6.</t>
-  </si>
-  <si>
-    <t>The module shall instansiate the Bit Timing Module as DUT7.</t>
   </si>
   <si>
     <t>TOP_INIT_02</t>
@@ -207,6 +183,30 @@
   </si>
   <si>
     <t>TOP_MAP_14</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Microcontroller Bus Interface as DUT0.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Configuration Registers as DUT1.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Tx FIFO as DUT2.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Rx FIFO as DUT3.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Tx Priority Logic as DUT4.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Acceptance Filter as DUT5.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Bit Stream Processor as DUT6.</t>
+  </si>
+  <si>
+    <t>The module shall instantiate the Bit Timing Module as DUT7.</t>
   </si>
 </sst>
 </file>
@@ -428,17 +428,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -454,12 +445,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,6 +461,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,7 +793,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,243 +805,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
+      <c r="D10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="17" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="17" t="s">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>